<commit_message>
Added to Browsing Page + LFP Testing Results Sheet
Just added some stuff to the browsing page, fixed up the map view. Updated my diary and transcribed LFP testing results into excel sheet.
</commit_message>
<xml_diff>
--- a/Documents/Oisin_Workspace/MScVault/Master's Project/UX Work/User Testing/UserTestingSpreadsheet.xlsx
+++ b/Documents/Oisin_Workspace/MScVault/Master's Project/UX Work/User Testing/UserTestingSpreadsheet.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oisin\Documents\GitHub\mscfinalproject\Documents\Oisin_Workspace\MScVault\Master's Project\UX Work\User Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1CC19E-45ED-45B8-A766-F254C0DF0BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB586A0-DB3E-4EBE-92E1-4BC9C014BC7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="-16200" windowWidth="14610" windowHeight="15585" xr2:uid="{1ED49114-756C-4824-AF04-6F492C704291}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1ED49114-756C-4824-AF04-6F492C704291}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="HME" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>SEQUENCE</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>Particpant 4</t>
-  </si>
-  <si>
-    <t>Participant 5</t>
   </si>
   <si>
     <t>Please Open Up the Search Filters:
@@ -166,6 +163,76 @@
   <si>
     <t>Select the Search Again
 On a scale of 1-5, rate how difficult it was to complete the task</t>
+  </si>
+  <si>
+    <t>GENERAL COMMENTS</t>
+  </si>
+  <si>
+    <t>Active Tags was not clear</t>
+  </si>
+  <si>
+    <t>Could not find favorites button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Once the user had established what the different </t>
+  </si>
+  <si>
+    <t>Feedback</t>
+  </si>
+  <si>
+    <t>Didn't recognize the search icon</t>
+  </si>
+  <si>
+    <t>Test Comments</t>
+  </si>
+  <si>
+    <t>No issues</t>
+  </si>
+  <si>
+    <t>No problems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Looks good, generally user friendly.
+- raise the apply and favorites button further up on the screen and make them bigger
+- want tags that are visible to be relevant to the user
+- property highlight tags are a bit ambiguous in their meaning, might be worthwhile having a popover to explain what the tag means
+- make thumbnail carousel to indicate more pictures
+- heat maps for different features on map
+</t>
+  </si>
+  <si>
+    <t>Need better color distinction for active tags</t>
+  </si>
+  <si>
+    <t>favorites (top) button could be made bigger</t>
+  </si>
+  <si>
+    <t>Saw the upper favorite button first, didn't see the bottom button, need to move the bottom button higher
+Main menu Button was hard to find, became easier after learning what it was</t>
+  </si>
+  <si>
+    <t>Make the apply button bigger and have it at the top</t>
+  </si>
+  <si>
+    <t>Save search icon doesn't match association</t>
+  </si>
+  <si>
+    <t>Want search bar to stand out more from the background on the landing page, make it larger + change its color
+Make buttons and text clearer and more visible
+Make the active tags larger + more distinct from the background</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Could not find the Favorites button, outside the 'F' shape for scanning
+Have menu beside the </t>
+  </si>
+  <si>
+    <t>Move the apply button up top, the contrast + color are good tho
+Complete later button needs to change to look more like a button
+Divider was good for making the button distinct in the edit applications page</t>
+  </si>
+  <si>
+    <t>make the picture grey instead for landing page
+save search icon doesn't match association, worthwhile to do A/B testing for icons</t>
   </si>
 </sst>
 </file>
@@ -243,7 +310,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -275,50 +342,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -634,187 +813,600 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8BBED7E-47F9-44F3-9F56-333A903D3CD0}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="43.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24" style="1" customWidth="1"/>
-    <col min="6" max="6" width="40.7109375" style="1" customWidth="1"/>
-    <col min="7" max="8" width="34.28515625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="55.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="19" style="18" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="24" style="6" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" style="6" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+    </row>
+    <row r="3" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+    </row>
+    <row r="4" spans="1:5" s="8" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="8">
+        <v>1</v>
+      </c>
+      <c r="D4" s="8">
+        <v>1</v>
+      </c>
+      <c r="E4" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="8" customFormat="1" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="8">
+        <v>2</v>
+      </c>
+      <c r="D5" s="8">
+        <v>1</v>
+      </c>
+      <c r="E5" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="8" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="8">
+        <v>1</v>
+      </c>
+      <c r="D6" s="8">
+        <v>1</v>
+      </c>
+      <c r="E6" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="8" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="8">
+        <v>2</v>
+      </c>
+      <c r="D7" s="8">
+        <v>2</v>
+      </c>
+      <c r="E7" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="8" customFormat="1" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="5" customFormat="1" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+    </row>
+    <row r="11" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="21"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+    </row>
+    <row r="12" spans="1:5" s="10" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="4" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="7" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+      <c r="C12" s="10">
+        <v>1</v>
+      </c>
+      <c r="D12" s="10">
+        <v>1</v>
+      </c>
+      <c r="E12" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="10" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" s="7" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="B13" s="2">
+        <v>5</v>
+      </c>
+      <c r="C13" s="10">
+        <v>2</v>
+      </c>
+      <c r="D13" s="10">
+        <v>2</v>
+      </c>
+      <c r="E13" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="10" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" s="7" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="10">
+        <v>3</v>
+      </c>
+      <c r="D14" s="10">
+        <v>2</v>
+      </c>
+      <c r="E14" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="10" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" s="7" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="10">
+        <v>1</v>
+      </c>
+      <c r="D15" s="10">
+        <v>1</v>
+      </c>
+      <c r="E15" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="10" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+      <c r="C16" s="10">
+        <v>1</v>
+      </c>
+      <c r="D16" s="10">
+        <v>1</v>
+      </c>
+      <c r="E16" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="10" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" s="10">
+        <v>1</v>
+      </c>
+      <c r="D17" s="10">
+        <v>1</v>
+      </c>
+      <c r="E17" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="10" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="10">
+        <v>1</v>
+      </c>
+      <c r="D18" s="10">
+        <v>1</v>
+      </c>
+      <c r="E18" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="15" customFormat="1" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+    </row>
+    <row r="21" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+      <c r="B21" s="23"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+    </row>
+    <row r="22" spans="1:5" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" s="10" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="B22" s="3">
+        <v>1</v>
+      </c>
+      <c r="C22" s="12">
+        <v>1</v>
+      </c>
+      <c r="D22" s="12">
+        <v>1</v>
+      </c>
+      <c r="E22" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" s="10" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
+      <c r="C23" s="12">
+        <v>2</v>
+      </c>
+      <c r="D23" s="12">
+        <v>2</v>
+      </c>
+      <c r="E23" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" s="10" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="B24" s="3">
+        <v>1</v>
+      </c>
+      <c r="C24" s="12">
+        <v>1</v>
+      </c>
+      <c r="D24" s="12">
+        <v>1</v>
+      </c>
+      <c r="E24" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" s="10" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+      <c r="C25" s="12">
+        <v>1</v>
+      </c>
+      <c r="D25" s="12">
+        <v>1</v>
+      </c>
+      <c r="E25" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" s="10" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="B26" s="3">
+        <v>1</v>
+      </c>
+      <c r="C26" s="12">
+        <v>1</v>
+      </c>
+      <c r="D26" s="12">
+        <v>1</v>
+      </c>
+      <c r="E26" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" s="10" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+      <c r="B27" s="3">
+        <v>1</v>
+      </c>
+      <c r="C27" s="12">
+        <v>1</v>
+      </c>
+      <c r="D27" s="12">
+        <v>1</v>
+      </c>
+      <c r="E27" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="16" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+    </row>
+    <row r="30" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+      <c r="B30" s="25"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+    </row>
+    <row r="31" spans="1:5" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" s="13" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
+      <c r="B31" s="4">
+        <v>1</v>
+      </c>
+      <c r="C31" s="14">
+        <v>1</v>
+      </c>
+      <c r="D31" s="14">
+        <v>1</v>
+      </c>
+      <c r="E31" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" s="13" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
+      <c r="B32" s="4">
+        <v>1</v>
+      </c>
+      <c r="C32" s="14">
+        <v>1</v>
+      </c>
+      <c r="D32" s="14">
+        <v>1</v>
+      </c>
+      <c r="E32" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" s="13" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
+      <c r="B33" s="4">
+        <v>1</v>
+      </c>
+      <c r="C33" s="14">
+        <v>1</v>
+      </c>
+      <c r="D33" s="14">
+        <v>1</v>
+      </c>
+      <c r="E33" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" s="13" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
+      <c r="B34" s="4">
+        <v>5</v>
+      </c>
+      <c r="C34" s="14">
+        <v>4</v>
+      </c>
+      <c r="D34" s="14">
+        <v>4</v>
+      </c>
+      <c r="E34" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" s="13" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
+      <c r="B35" s="4">
+        <v>1</v>
+      </c>
+      <c r="C35" s="14">
+        <v>1</v>
+      </c>
+      <c r="D35" s="14">
+        <v>1</v>
+      </c>
+      <c r="E35" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" s="13" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A33" s="12" t="s">
+      <c r="B36" s="4">
+        <v>1</v>
+      </c>
+      <c r="C36" s="14">
+        <v>1</v>
+      </c>
+      <c r="D36" s="14">
+        <v>1</v>
+      </c>
+      <c r="E36" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" s="13" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A34" s="12" t="s">
+      <c r="B37" s="4">
+        <v>1</v>
+      </c>
+      <c r="C37" s="14">
+        <v>1</v>
+      </c>
+      <c r="D37" s="14">
+        <v>1</v>
+      </c>
+      <c r="E37" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="17" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="17" t="s">
         <v>34</v>
+      </c>
+      <c r="B38" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="E38" s="34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="291" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Redeploying to New Region
Had to Redeploy to new region
</commit_message>
<xml_diff>
--- a/Documents/Oisin_Workspace/MScVault/Master's Project/UX Work/User Testing/UserTestingSpreadsheet.xlsx
+++ b/Documents/Oisin_Workspace/MScVault/Master's Project/UX Work/User Testing/UserTestingSpreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oisin\Documents\GitHub\mscfinalproject\Documents\Oisin_Workspace\MScVault\Master's Project\UX Work\User Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB586A0-DB3E-4EBE-92E1-4BC9C014BC7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD0B016-516C-4F5C-A03C-06AEAB55B359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1ED49114-756C-4824-AF04-6F492C704291}"/>
+    <workbookView xWindow="-109" yWindow="-14780" windowWidth="26301" windowHeight="14169" xr2:uid="{1ED49114-756C-4824-AF04-6F492C704291}"/>
   </bookViews>
   <sheets>
     <sheet name="HME" sheetId="1" r:id="rId1"/>
@@ -395,7 +395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -409,7 +409,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -439,13 +439,13 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -476,21 +476,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -815,22 +800,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8BBED7E-47F9-44F3-9F56-333A903D3CD0}">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.42578125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="55.375" style="6" customWidth="1"/>
     <col min="2" max="2" width="19" style="18" customWidth="1"/>
-    <col min="3" max="3" width="35.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="35.25" style="6" customWidth="1"/>
     <col min="4" max="4" width="24" style="6" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="34.28515625" style="6" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="6"/>
+    <col min="5" max="5" width="40.75" style="6" customWidth="1"/>
+    <col min="6" max="6" width="34.25" style="6" customWidth="1"/>
+    <col min="7" max="16384" width="9.125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.95" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -847,19 +830,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-    </row>
-    <row r="3" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.95" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:5" s="7" customFormat="1" ht="14.95" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="19"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
     </row>
     <row r="4" spans="1:5" s="8" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -895,7 +871,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="8" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="8" customFormat="1" ht="84.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -912,7 +888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="8" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="8" customFormat="1" ht="80.349999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -946,7 +922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="5" customFormat="1" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="5" customFormat="1" ht="122.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>34</v>
       </c>
@@ -962,22 +938,14 @@
       <c r="E9" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
     </row>
     <row r="11" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="21"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-    </row>
-    <row r="12" spans="1:5" s="10" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:5" s="10" customFormat="1" ht="69.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -994,7 +962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="10" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" s="10" customFormat="1" ht="66.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -1011,7 +979,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="10" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" s="10" customFormat="1" ht="73.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1028,7 +996,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="10" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" s="10" customFormat="1" ht="80.349999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1045,7 +1013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="10" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" s="10" customFormat="1" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -1062,7 +1030,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="10" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" s="10" customFormat="1" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -1079,7 +1047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="10" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" s="10" customFormat="1" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
@@ -1096,7 +1064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="15" customFormat="1" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" s="15" customFormat="1" ht="159.80000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>34</v>
       </c>
@@ -1112,22 +1080,14 @@
       <c r="E19" s="15" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
     </row>
     <row r="21" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="23"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-    </row>
-    <row r="22" spans="1:5" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:5" s="12" customFormat="1" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -1144,7 +1104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" s="12" customFormat="1" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
@@ -1161,7 +1121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" s="12" customFormat="1" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
@@ -1178,7 +1138,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" s="12" customFormat="1" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
@@ -1195,7 +1155,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" s="12" customFormat="1" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
@@ -1212,7 +1172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" s="12" customFormat="1" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>25</v>
       </c>
@@ -1246,21 +1206,13 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
-    </row>
     <row r="30" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>26</v>
       </c>
       <c r="B30" s="25"/>
-      <c r="C30" s="32"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="32"/>
-    </row>
-    <row r="31" spans="1:5" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:5" s="14" customFormat="1" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>27</v>
       </c>
@@ -1277,7 +1229,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" s="14" customFormat="1" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>28</v>
       </c>
@@ -1294,7 +1246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" s="14" customFormat="1" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>29</v>
       </c>
@@ -1311,7 +1263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" s="14" customFormat="1" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>30</v>
       </c>
@@ -1328,7 +1280,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" s="14" customFormat="1" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>31</v>
       </c>
@@ -1345,7 +1297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" s="14" customFormat="1" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>32</v>
       </c>
@@ -1362,7 +1314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" s="14" customFormat="1" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>33</v>
       </c>
@@ -1379,24 +1331,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="17" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" s="17" customFormat="1" ht="105.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="33" t="s">
+      <c r="B38" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="33" t="s">
+      <c r="C38" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="D38" s="34" t="s">
+      <c r="D38" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="E38" s="34" t="s">
+      <c r="E38" s="29" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="291" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="291.10000000000002" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>38</v>
       </c>

</xml_diff>